<commit_message>
fix: refresh reten baru, fix semua branding giret. BISMILLAH ALLAH MAHA BESAR. LETS GO
</commit_message>
<xml_diff>
--- a/public/exports/Reten BPE Perio.xlsx
+++ b/public/exports/Reten BPE Perio.xlsx
@@ -581,7 +581,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="77">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -654,9 +654,6 @@
     </xf>
     <xf borderId="13" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="14" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" textRotation="90" wrapText="1"/>
-    </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
@@ -676,23 +673,20 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="12" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="22" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" textRotation="90" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" textRotation="90" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" textRotation="90" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" textRotation="90" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="7" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="23" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" textRotation="90" wrapText="1"/>
+      <alignment horizontal="center" shrinkToFit="0" textRotation="90" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="23" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" textRotation="90"/>
+      <alignment horizontal="center" textRotation="90" vertical="center"/>
     </xf>
     <xf borderId="24" fillId="0" fontId="6" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1616,34 +1610,34 @@
       </c>
       <c r="AE13" s="25"/>
       <c r="AF13" s="26"/>
-      <c r="AG13" s="30" t="s">
+      <c r="AG13" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="AH13" s="30" t="s">
+      <c r="AH13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="AI13" s="30" t="s">
+      <c r="AI13" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="AJ13" s="31"/>
-      <c r="AK13" s="31"/>
-      <c r="AL13" s="31"/>
-      <c r="AM13" s="31"/>
-      <c r="AN13" s="31"/>
-      <c r="AO13" s="31"/>
-      <c r="AP13" s="31"/>
+      <c r="AJ13" s="30"/>
+      <c r="AK13" s="30"/>
+      <c r="AL13" s="30"/>
+      <c r="AM13" s="30"/>
+      <c r="AN13" s="30"/>
+      <c r="AO13" s="30"/>
+      <c r="AP13" s="30"/>
     </row>
     <row r="14" ht="30.0" customHeight="1">
       <c r="A14" s="1"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="32"/>
-      <c r="D14" s="33"/>
-      <c r="E14" s="34"/>
-      <c r="G14" s="35"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="38"/>
-      <c r="K14" s="39" t="s">
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+      <c r="G14" s="34"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="37"/>
+      <c r="K14" s="38" t="s">
         <v>20</v>
       </c>
       <c r="L14" s="28"/>
@@ -1653,12 +1647,12 @@
       <c r="P14" s="28"/>
       <c r="Q14" s="28"/>
       <c r="R14" s="28"/>
-      <c r="S14" s="40" t="s">
+      <c r="S14" s="39" t="s">
         <v>21</v>
       </c>
       <c r="T14" s="28"/>
       <c r="U14" s="29"/>
-      <c r="V14" s="40" t="s">
+      <c r="V14" s="39" t="s">
         <v>22</v>
       </c>
       <c r="W14" s="28"/>
@@ -1667,45 +1661,45 @@
       <c r="Z14" s="28"/>
       <c r="AA14" s="28"/>
       <c r="AB14" s="29"/>
-      <c r="AC14" s="30" t="s">
+      <c r="AC14" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="AD14" s="36"/>
-      <c r="AE14" s="37"/>
-      <c r="AF14" s="38"/>
-      <c r="AG14" s="32"/>
-      <c r="AH14" s="32"/>
-      <c r="AI14" s="32"/>
-      <c r="AJ14" s="41"/>
-      <c r="AK14" s="41"/>
-      <c r="AL14" s="41"/>
-      <c r="AM14" s="41"/>
-      <c r="AN14" s="41"/>
-      <c r="AO14" s="41"/>
-      <c r="AP14" s="41"/>
+      <c r="AD14" s="35"/>
+      <c r="AE14" s="36"/>
+      <c r="AF14" s="37"/>
+      <c r="AG14" s="31"/>
+      <c r="AH14" s="31"/>
+      <c r="AI14" s="31"/>
+      <c r="AJ14" s="40"/>
+      <c r="AK14" s="40"/>
+      <c r="AL14" s="40"/>
+      <c r="AM14" s="40"/>
+      <c r="AN14" s="40"/>
+      <c r="AO14" s="40"/>
+      <c r="AP14" s="40"/>
     </row>
     <row r="15" ht="21.0" customHeight="1">
       <c r="A15" s="1"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
-      <c r="D15" s="33"/>
-      <c r="E15" s="42" t="s">
+      <c r="B15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="38" t="s">
         <v>24</v>
       </c>
       <c r="F15" s="29"/>
-      <c r="G15" s="30" t="s">
+      <c r="G15" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="H15" s="43" t="s">
+      <c r="H15" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="I15" s="30" t="s">
+      <c r="I15" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="30" t="s">
+      <c r="J15" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="39" t="s">
+      <c r="K15" s="38" t="s">
         <v>28</v>
       </c>
       <c r="L15" s="28"/>
@@ -1715,467 +1709,467 @@
       <c r="P15" s="28"/>
       <c r="Q15" s="28"/>
       <c r="R15" s="29"/>
-      <c r="S15" s="30" t="s">
+      <c r="S15" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="T15" s="30" t="s">
+      <c r="T15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="U15" s="30" t="s">
+      <c r="U15" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="V15" s="44" t="s">
+      <c r="V15" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="W15" s="30" t="s">
+      <c r="W15" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="X15" s="30" t="s">
+      <c r="X15" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="Y15" s="30" t="s">
+      <c r="Y15" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="Z15" s="30" t="s">
+      <c r="Z15" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="AA15" s="30" t="s">
+      <c r="AA15" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="AB15" s="30" t="s">
+      <c r="AB15" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="AC15" s="32"/>
-      <c r="AD15" s="45" t="s">
+      <c r="AC15" s="31"/>
+      <c r="AD15" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="AE15" s="39" t="s">
+      <c r="AE15" s="38" t="s">
         <v>39</v>
       </c>
       <c r="AF15" s="29"/>
-      <c r="AG15" s="32"/>
-      <c r="AH15" s="32"/>
-      <c r="AI15" s="32"/>
-      <c r="AJ15" s="31"/>
-      <c r="AK15" s="31"/>
-      <c r="AL15" s="31"/>
-      <c r="AM15" s="31"/>
-      <c r="AN15" s="31"/>
-      <c r="AO15" s="31"/>
-      <c r="AP15" s="41"/>
+      <c r="AG15" s="31"/>
+      <c r="AH15" s="31"/>
+      <c r="AI15" s="31"/>
+      <c r="AJ15" s="30"/>
+      <c r="AK15" s="30"/>
+      <c r="AL15" s="30"/>
+      <c r="AM15" s="30"/>
+      <c r="AN15" s="30"/>
+      <c r="AO15" s="30"/>
+      <c r="AP15" s="40"/>
     </row>
     <row r="16" ht="68.25" customHeight="1">
       <c r="A16" s="1"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="32"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="46" t="s">
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="44" t="s">
         <v>40</v>
       </c>
-      <c r="F16" s="47" t="s">
+      <c r="F16" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="32"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="32"/>
-      <c r="J16" s="32"/>
-      <c r="K16" s="30" t="s">
+      <c r="G16" s="31"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="L16" s="49" t="s">
+      <c r="L16" s="47" t="s">
         <v>42</v>
       </c>
       <c r="M16" s="28"/>
       <c r="N16" s="29"/>
-      <c r="O16" s="49" t="s">
+      <c r="O16" s="47" t="s">
         <v>43</v>
       </c>
       <c r="P16" s="29"/>
-      <c r="Q16" s="50" t="s">
+      <c r="Q16" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="R16" s="50" t="s">
+      <c r="R16" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="S16" s="32"/>
-      <c r="T16" s="32"/>
-      <c r="U16" s="32"/>
-      <c r="V16" s="32"/>
-      <c r="W16" s="32"/>
-      <c r="X16" s="32"/>
-      <c r="Y16" s="32"/>
-      <c r="Z16" s="32"/>
-      <c r="AA16" s="32"/>
-      <c r="AB16" s="32"/>
-      <c r="AC16" s="32"/>
-      <c r="AD16" s="32"/>
-      <c r="AE16" s="30" t="s">
+      <c r="S16" s="31"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="31"/>
+      <c r="W16" s="31"/>
+      <c r="X16" s="31"/>
+      <c r="Y16" s="31"/>
+      <c r="Z16" s="31"/>
+      <c r="AA16" s="31"/>
+      <c r="AB16" s="31"/>
+      <c r="AC16" s="31"/>
+      <c r="AD16" s="31"/>
+      <c r="AE16" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="AF16" s="30" t="s">
+      <c r="AF16" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="AG16" s="32"/>
-      <c r="AH16" s="32"/>
-      <c r="AI16" s="32"/>
-      <c r="AJ16" s="31"/>
-      <c r="AK16" s="31"/>
-      <c r="AL16" s="31"/>
-      <c r="AM16" s="31"/>
-      <c r="AN16" s="31"/>
-      <c r="AO16" s="31"/>
-      <c r="AP16" s="41"/>
+      <c r="AG16" s="31"/>
+      <c r="AH16" s="31"/>
+      <c r="AI16" s="31"/>
+      <c r="AJ16" s="30"/>
+      <c r="AK16" s="30"/>
+      <c r="AL16" s="30"/>
+      <c r="AM16" s="30"/>
+      <c r="AN16" s="30"/>
+      <c r="AO16" s="30"/>
+      <c r="AP16" s="40"/>
     </row>
     <row r="17" ht="52.5" customHeight="1">
       <c r="A17" s="1"/>
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="51"/>
-      <c r="H17" s="53"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="54">
+      <c r="B17" s="49"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="52">
         <v>0.0</v>
       </c>
-      <c r="M17" s="54">
+      <c r="M17" s="52">
         <v>1.0</v>
       </c>
-      <c r="N17" s="54">
+      <c r="N17" s="52">
         <v>2.0</v>
       </c>
-      <c r="O17" s="54">
+      <c r="O17" s="52">
         <v>3.0</v>
       </c>
-      <c r="P17" s="54">
+      <c r="P17" s="52">
         <v>4.0</v>
       </c>
-      <c r="Q17" s="54" t="s">
+      <c r="Q17" s="52" t="s">
         <v>47</v>
       </c>
-      <c r="R17" s="55" t="s">
+      <c r="R17" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="S17" s="51"/>
-      <c r="T17" s="51"/>
-      <c r="U17" s="51"/>
-      <c r="V17" s="51"/>
-      <c r="W17" s="51"/>
-      <c r="X17" s="51"/>
-      <c r="Y17" s="51"/>
-      <c r="Z17" s="51"/>
-      <c r="AA17" s="51"/>
-      <c r="AB17" s="51"/>
-      <c r="AC17" s="51"/>
-      <c r="AD17" s="51"/>
-      <c r="AE17" s="51"/>
-      <c r="AF17" s="51"/>
-      <c r="AG17" s="51"/>
-      <c r="AH17" s="51"/>
-      <c r="AI17" s="51"/>
-      <c r="AJ17" s="31"/>
-      <c r="AK17" s="31"/>
-      <c r="AL17" s="31"/>
-      <c r="AM17" s="31"/>
-      <c r="AN17" s="31"/>
-      <c r="AO17" s="31"/>
-      <c r="AP17" s="41"/>
+      <c r="S17" s="49"/>
+      <c r="T17" s="49"/>
+      <c r="U17" s="49"/>
+      <c r="V17" s="49"/>
+      <c r="W17" s="49"/>
+      <c r="X17" s="49"/>
+      <c r="Y17" s="49"/>
+      <c r="Z17" s="49"/>
+      <c r="AA17" s="49"/>
+      <c r="AB17" s="49"/>
+      <c r="AC17" s="49"/>
+      <c r="AD17" s="49"/>
+      <c r="AE17" s="49"/>
+      <c r="AF17" s="49"/>
+      <c r="AG17" s="49"/>
+      <c r="AH17" s="49"/>
+      <c r="AI17" s="49"/>
+      <c r="AJ17" s="30"/>
+      <c r="AK17" s="30"/>
+      <c r="AL17" s="30"/>
+      <c r="AM17" s="30"/>
+      <c r="AN17" s="30"/>
+      <c r="AO17" s="30"/>
+      <c r="AP17" s="40"/>
     </row>
     <row r="18" ht="19.5" customHeight="1">
       <c r="A18" s="1"/>
-      <c r="B18" s="56">
+      <c r="B18" s="54">
         <v>3.0</v>
       </c>
-      <c r="C18" s="57">
+      <c r="C18" s="55">
         <v>4.0</v>
       </c>
-      <c r="D18" s="57">
+      <c r="D18" s="55">
         <v>5.0</v>
       </c>
-      <c r="E18" s="57">
+      <c r="E18" s="55">
         <v>6.0</v>
       </c>
-      <c r="F18" s="57">
+      <c r="F18" s="55">
         <v>7.0</v>
       </c>
-      <c r="G18" s="57">
+      <c r="G18" s="55">
         <v>8.0</v>
       </c>
-      <c r="H18" s="57">
+      <c r="H18" s="55">
         <v>9.0</v>
       </c>
-      <c r="I18" s="57">
+      <c r="I18" s="55">
         <v>10.0</v>
       </c>
-      <c r="J18" s="57">
+      <c r="J18" s="55">
         <v>11.0</v>
       </c>
-      <c r="K18" s="57">
+      <c r="K18" s="55">
         <v>12.0</v>
       </c>
-      <c r="L18" s="57">
+      <c r="L18" s="55">
         <v>13.0</v>
       </c>
-      <c r="M18" s="57">
+      <c r="M18" s="55">
         <v>14.0</v>
       </c>
-      <c r="N18" s="57">
+      <c r="N18" s="55">
         <v>15.0</v>
       </c>
-      <c r="O18" s="57">
+      <c r="O18" s="55">
         <v>16.0</v>
       </c>
-      <c r="P18" s="57">
+      <c r="P18" s="55">
         <v>17.0</v>
       </c>
-      <c r="Q18" s="57">
+      <c r="Q18" s="55">
         <v>18.0</v>
       </c>
-      <c r="R18" s="57">
+      <c r="R18" s="55">
         <v>19.0</v>
       </c>
-      <c r="S18" s="57">
+      <c r="S18" s="55">
         <v>20.0</v>
       </c>
-      <c r="T18" s="57">
+      <c r="T18" s="55">
         <v>21.0</v>
       </c>
-      <c r="U18" s="57">
+      <c r="U18" s="55">
         <v>22.0</v>
       </c>
-      <c r="V18" s="57">
+      <c r="V18" s="55">
         <v>23.0</v>
       </c>
-      <c r="W18" s="57">
+      <c r="W18" s="55">
         <v>24.0</v>
       </c>
-      <c r="X18" s="57">
+      <c r="X18" s="55">
         <v>25.0</v>
       </c>
-      <c r="Y18" s="57">
+      <c r="Y18" s="55">
         <v>26.0</v>
       </c>
-      <c r="Z18" s="57">
+      <c r="Z18" s="55">
         <v>27.0</v>
       </c>
-      <c r="AA18" s="57">
+      <c r="AA18" s="55">
         <v>28.0</v>
       </c>
-      <c r="AB18" s="57">
+      <c r="AB18" s="55">
         <v>29.0</v>
       </c>
-      <c r="AC18" s="57">
+      <c r="AC18" s="55">
         <v>30.0</v>
       </c>
-      <c r="AD18" s="57">
+      <c r="AD18" s="55">
         <v>31.0</v>
       </c>
-      <c r="AE18" s="57">
+      <c r="AE18" s="55">
         <v>32.0</v>
       </c>
-      <c r="AF18" s="57">
+      <c r="AF18" s="55">
         <v>33.0</v>
       </c>
-      <c r="AG18" s="57">
+      <c r="AG18" s="55">
         <v>34.0</v>
       </c>
-      <c r="AH18" s="57">
+      <c r="AH18" s="55">
         <v>35.0</v>
       </c>
-      <c r="AI18" s="57">
+      <c r="AI18" s="55">
         <v>36.0</v>
       </c>
-      <c r="AJ18" s="58"/>
-      <c r="AK18" s="41"/>
-      <c r="AL18" s="41"/>
-      <c r="AM18" s="41"/>
-      <c r="AN18" s="41"/>
-      <c r="AO18" s="41"/>
-      <c r="AP18" s="41"/>
+      <c r="AJ18" s="56"/>
+      <c r="AK18" s="40"/>
+      <c r="AL18" s="40"/>
+      <c r="AM18" s="40"/>
+      <c r="AN18" s="40"/>
+      <c r="AO18" s="40"/>
+      <c r="AP18" s="40"/>
     </row>
     <row r="19" ht="19.5" customHeight="1">
       <c r="A19" s="1"/>
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="57" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="60" t="s">
+      <c r="C19" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="57"/>
-      <c r="P19" s="57"/>
-      <c r="Q19" s="57"/>
-      <c r="R19" s="57"/>
-      <c r="S19" s="57"/>
-      <c r="T19" s="57"/>
-      <c r="U19" s="57"/>
-      <c r="V19" s="57"/>
-      <c r="W19" s="57"/>
-      <c r="X19" s="57"/>
-      <c r="Y19" s="57"/>
-      <c r="Z19" s="57"/>
-      <c r="AA19" s="57"/>
-      <c r="AB19" s="57"/>
-      <c r="AC19" s="57"/>
-      <c r="AD19" s="57"/>
-      <c r="AE19" s="57"/>
-      <c r="AF19" s="57"/>
-      <c r="AG19" s="57"/>
-      <c r="AH19" s="57"/>
-      <c r="AI19" s="57"/>
-      <c r="AJ19" s="41"/>
-      <c r="AK19" s="41"/>
-      <c r="AL19" s="41"/>
-      <c r="AM19" s="41"/>
-      <c r="AN19" s="41"/>
-      <c r="AO19" s="41"/>
-      <c r="AP19" s="41"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="55"/>
+      <c r="K19" s="54"/>
+      <c r="L19" s="54"/>
+      <c r="M19" s="54"/>
+      <c r="N19" s="54"/>
+      <c r="O19" s="55"/>
+      <c r="P19" s="55"/>
+      <c r="Q19" s="55"/>
+      <c r="R19" s="55"/>
+      <c r="S19" s="55"/>
+      <c r="T19" s="55"/>
+      <c r="U19" s="55"/>
+      <c r="V19" s="55"/>
+      <c r="W19" s="55"/>
+      <c r="X19" s="55"/>
+      <c r="Y19" s="55"/>
+      <c r="Z19" s="55"/>
+      <c r="AA19" s="55"/>
+      <c r="AB19" s="55"/>
+      <c r="AC19" s="55"/>
+      <c r="AD19" s="55"/>
+      <c r="AE19" s="55"/>
+      <c r="AF19" s="55"/>
+      <c r="AG19" s="55"/>
+      <c r="AH19" s="55"/>
+      <c r="AI19" s="55"/>
+      <c r="AJ19" s="40"/>
+      <c r="AK19" s="40"/>
+      <c r="AL19" s="40"/>
+      <c r="AM19" s="40"/>
+      <c r="AN19" s="40"/>
+      <c r="AO19" s="40"/>
+      <c r="AP19" s="40"/>
     </row>
     <row r="20" ht="19.5" customHeight="1">
       <c r="A20" s="1"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="60" t="s">
+      <c r="B20" s="49"/>
+      <c r="C20" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="56"/>
-      <c r="G20" s="57"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="57"/>
-      <c r="J20" s="57"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="57"/>
-      <c r="P20" s="57"/>
-      <c r="Q20" s="57"/>
-      <c r="R20" s="57"/>
-      <c r="S20" s="57"/>
-      <c r="T20" s="57"/>
-      <c r="U20" s="57"/>
-      <c r="V20" s="57"/>
-      <c r="W20" s="57"/>
-      <c r="X20" s="57"/>
-      <c r="Y20" s="57"/>
-      <c r="Z20" s="57"/>
-      <c r="AA20" s="57"/>
-      <c r="AB20" s="57"/>
-      <c r="AC20" s="57"/>
-      <c r="AD20" s="57"/>
-      <c r="AE20" s="57"/>
-      <c r="AF20" s="57"/>
-      <c r="AG20" s="57"/>
-      <c r="AH20" s="57"/>
-      <c r="AI20" s="57"/>
-      <c r="AJ20" s="41"/>
-      <c r="AK20" s="41"/>
-      <c r="AL20" s="41"/>
-      <c r="AM20" s="41"/>
-      <c r="AN20" s="41"/>
-      <c r="AO20" s="41"/>
-      <c r="AP20" s="41"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="54"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="55"/>
+      <c r="J20" s="55"/>
+      <c r="K20" s="54"/>
+      <c r="L20" s="54"/>
+      <c r="M20" s="54"/>
+      <c r="N20" s="54"/>
+      <c r="O20" s="55"/>
+      <c r="P20" s="55"/>
+      <c r="Q20" s="55"/>
+      <c r="R20" s="55"/>
+      <c r="S20" s="55"/>
+      <c r="T20" s="55"/>
+      <c r="U20" s="55"/>
+      <c r="V20" s="55"/>
+      <c r="W20" s="55"/>
+      <c r="X20" s="55"/>
+      <c r="Y20" s="55"/>
+      <c r="Z20" s="55"/>
+      <c r="AA20" s="55"/>
+      <c r="AB20" s="55"/>
+      <c r="AC20" s="55"/>
+      <c r="AD20" s="55"/>
+      <c r="AE20" s="55"/>
+      <c r="AF20" s="55"/>
+      <c r="AG20" s="55"/>
+      <c r="AH20" s="55"/>
+      <c r="AI20" s="55"/>
+      <c r="AJ20" s="40"/>
+      <c r="AK20" s="40"/>
+      <c r="AL20" s="40"/>
+      <c r="AM20" s="40"/>
+      <c r="AN20" s="40"/>
+      <c r="AO20" s="40"/>
+      <c r="AP20" s="40"/>
     </row>
     <row r="21" ht="19.5" customHeight="1">
       <c r="A21" s="1"/>
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="60" t="s">
+      <c r="C21" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="60"/>
-      <c r="F21" s="60"/>
-      <c r="G21" s="56"/>
-      <c r="H21" s="56"/>
-      <c r="I21" s="56"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="57"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="57"/>
-      <c r="O21" s="56"/>
-      <c r="P21" s="57"/>
-      <c r="Q21" s="57"/>
-      <c r="R21" s="57"/>
-      <c r="S21" s="56"/>
-      <c r="T21" s="57"/>
-      <c r="U21" s="56"/>
-      <c r="V21" s="57"/>
-      <c r="W21" s="57"/>
-      <c r="X21" s="57"/>
-      <c r="Y21" s="57"/>
-      <c r="Z21" s="57"/>
-      <c r="AA21" s="57"/>
-      <c r="AB21" s="57"/>
-      <c r="AC21" s="57"/>
-      <c r="AD21" s="57"/>
-      <c r="AE21" s="57"/>
-      <c r="AF21" s="56"/>
-      <c r="AG21" s="57"/>
-      <c r="AH21" s="56"/>
-      <c r="AI21" s="57"/>
-      <c r="AJ21" s="41"/>
-      <c r="AK21" s="41"/>
-      <c r="AL21" s="41"/>
-      <c r="AM21" s="41"/>
-      <c r="AN21" s="41"/>
-      <c r="AO21" s="41"/>
-      <c r="AP21" s="41"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="54"/>
+      <c r="I21" s="54"/>
+      <c r="J21" s="54"/>
+      <c r="K21" s="54"/>
+      <c r="L21" s="55"/>
+      <c r="M21" s="54"/>
+      <c r="N21" s="55"/>
+      <c r="O21" s="54"/>
+      <c r="P21" s="55"/>
+      <c r="Q21" s="55"/>
+      <c r="R21" s="55"/>
+      <c r="S21" s="54"/>
+      <c r="T21" s="55"/>
+      <c r="U21" s="54"/>
+      <c r="V21" s="55"/>
+      <c r="W21" s="55"/>
+      <c r="X21" s="55"/>
+      <c r="Y21" s="55"/>
+      <c r="Z21" s="55"/>
+      <c r="AA21" s="55"/>
+      <c r="AB21" s="55"/>
+      <c r="AC21" s="55"/>
+      <c r="AD21" s="55"/>
+      <c r="AE21" s="55"/>
+      <c r="AF21" s="54"/>
+      <c r="AG21" s="55"/>
+      <c r="AH21" s="54"/>
+      <c r="AI21" s="55"/>
+      <c r="AJ21" s="40"/>
+      <c r="AK21" s="40"/>
+      <c r="AL21" s="40"/>
+      <c r="AM21" s="40"/>
+      <c r="AN21" s="40"/>
+      <c r="AO21" s="40"/>
+      <c r="AP21" s="40"/>
     </row>
     <row r="22" ht="19.5" customHeight="1">
       <c r="A22" s="1"/>
-      <c r="B22" s="51"/>
-      <c r="C22" s="60" t="s">
+      <c r="B22" s="49"/>
+      <c r="C22" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="61"/>
-      <c r="H22" s="61"/>
-      <c r="I22" s="61"/>
-      <c r="J22" s="61"/>
-      <c r="K22" s="61"/>
-      <c r="L22" s="61"/>
-      <c r="M22" s="61"/>
-      <c r="N22" s="61"/>
-      <c r="O22" s="61"/>
-      <c r="P22" s="61"/>
-      <c r="Q22" s="61"/>
-      <c r="R22" s="61"/>
-      <c r="S22" s="62"/>
-      <c r="T22" s="62"/>
-      <c r="U22" s="62"/>
-      <c r="V22" s="62"/>
-      <c r="W22" s="62"/>
-      <c r="X22" s="62"/>
-      <c r="Y22" s="62"/>
-      <c r="Z22" s="62"/>
-      <c r="AA22" s="62"/>
-      <c r="AB22" s="62"/>
-      <c r="AC22" s="62"/>
-      <c r="AD22" s="62"/>
-      <c r="AE22" s="62"/>
-      <c r="AF22" s="62"/>
-      <c r="AG22" s="62"/>
-      <c r="AH22" s="62"/>
-      <c r="AI22" s="63"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="59"/>
+      <c r="H22" s="59"/>
+      <c r="I22" s="59"/>
+      <c r="J22" s="59"/>
+      <c r="K22" s="59"/>
+      <c r="L22" s="59"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="59"/>
+      <c r="P22" s="59"/>
+      <c r="Q22" s="59"/>
+      <c r="R22" s="59"/>
+      <c r="S22" s="60"/>
+      <c r="T22" s="60"/>
+      <c r="U22" s="60"/>
+      <c r="V22" s="60"/>
+      <c r="W22" s="60"/>
+      <c r="X22" s="60"/>
+      <c r="Y22" s="60"/>
+      <c r="Z22" s="60"/>
+      <c r="AA22" s="60"/>
+      <c r="AB22" s="60"/>
+      <c r="AC22" s="60"/>
+      <c r="AD22" s="60"/>
+      <c r="AE22" s="60"/>
+      <c r="AF22" s="60"/>
+      <c r="AG22" s="60"/>
+      <c r="AH22" s="60"/>
+      <c r="AI22" s="61"/>
       <c r="AJ22" s="1"/>
       <c r="AK22" s="1"/>
       <c r="AL22" s="1"/>
@@ -2186,44 +2180,44 @@
     </row>
     <row r="23" ht="19.5" customHeight="1">
       <c r="A23" s="1"/>
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="57" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="61"/>
-      <c r="J23" s="61"/>
-      <c r="K23" s="61"/>
-      <c r="L23" s="61"/>
-      <c r="M23" s="61"/>
-      <c r="N23" s="61"/>
-      <c r="O23" s="61"/>
-      <c r="P23" s="61"/>
-      <c r="Q23" s="61"/>
-      <c r="R23" s="61"/>
-      <c r="S23" s="62"/>
-      <c r="T23" s="62"/>
-      <c r="U23" s="62"/>
-      <c r="V23" s="62"/>
-      <c r="W23" s="62"/>
-      <c r="X23" s="62"/>
-      <c r="Y23" s="62"/>
-      <c r="Z23" s="62"/>
-      <c r="AA23" s="62"/>
-      <c r="AB23" s="62"/>
-      <c r="AC23" s="62"/>
-      <c r="AD23" s="62"/>
-      <c r="AE23" s="62"/>
-      <c r="AF23" s="62"/>
-      <c r="AG23" s="62"/>
-      <c r="AH23" s="62"/>
-      <c r="AI23" s="63"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="59"/>
+      <c r="P23" s="59"/>
+      <c r="Q23" s="59"/>
+      <c r="R23" s="59"/>
+      <c r="S23" s="60"/>
+      <c r="T23" s="60"/>
+      <c r="U23" s="60"/>
+      <c r="V23" s="60"/>
+      <c r="W23" s="60"/>
+      <c r="X23" s="60"/>
+      <c r="Y23" s="60"/>
+      <c r="Z23" s="60"/>
+      <c r="AA23" s="60"/>
+      <c r="AB23" s="60"/>
+      <c r="AC23" s="60"/>
+      <c r="AD23" s="60"/>
+      <c r="AE23" s="60"/>
+      <c r="AF23" s="60"/>
+      <c r="AG23" s="60"/>
+      <c r="AH23" s="60"/>
+      <c r="AI23" s="61"/>
       <c r="AJ23" s="1"/>
       <c r="AK23" s="1"/>
       <c r="AL23" s="1"/>
@@ -2234,42 +2228,42 @@
     </row>
     <row r="24" ht="19.5" customHeight="1">
       <c r="A24" s="1"/>
-      <c r="B24" s="51"/>
-      <c r="C24" s="60" t="s">
+      <c r="B24" s="49"/>
+      <c r="C24" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="D24" s="60"/>
-      <c r="E24" s="60"/>
-      <c r="F24" s="60"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="61"/>
-      <c r="J24" s="61"/>
-      <c r="K24" s="61"/>
-      <c r="L24" s="61"/>
-      <c r="M24" s="61"/>
-      <c r="N24" s="61"/>
-      <c r="O24" s="61"/>
-      <c r="P24" s="61"/>
-      <c r="Q24" s="61"/>
-      <c r="R24" s="61"/>
-      <c r="S24" s="62"/>
-      <c r="T24" s="62"/>
-      <c r="U24" s="62"/>
-      <c r="V24" s="62"/>
-      <c r="W24" s="62"/>
-      <c r="X24" s="62"/>
-      <c r="Y24" s="62"/>
-      <c r="Z24" s="62"/>
-      <c r="AA24" s="62"/>
-      <c r="AB24" s="62"/>
-      <c r="AC24" s="62"/>
-      <c r="AD24" s="62"/>
-      <c r="AE24" s="62"/>
-      <c r="AF24" s="62"/>
-      <c r="AG24" s="62"/>
-      <c r="AH24" s="62"/>
-      <c r="AI24" s="63"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="58"/>
+      <c r="F24" s="58"/>
+      <c r="G24" s="59"/>
+      <c r="H24" s="59"/>
+      <c r="I24" s="59"/>
+      <c r="J24" s="59"/>
+      <c r="K24" s="59"/>
+      <c r="L24" s="59"/>
+      <c r="M24" s="59"/>
+      <c r="N24" s="59"/>
+      <c r="O24" s="59"/>
+      <c r="P24" s="59"/>
+      <c r="Q24" s="59"/>
+      <c r="R24" s="59"/>
+      <c r="S24" s="60"/>
+      <c r="T24" s="60"/>
+      <c r="U24" s="60"/>
+      <c r="V24" s="60"/>
+      <c r="W24" s="60"/>
+      <c r="X24" s="60"/>
+      <c r="Y24" s="60"/>
+      <c r="Z24" s="60"/>
+      <c r="AA24" s="60"/>
+      <c r="AB24" s="60"/>
+      <c r="AC24" s="60"/>
+      <c r="AD24" s="60"/>
+      <c r="AE24" s="60"/>
+      <c r="AF24" s="60"/>
+      <c r="AG24" s="60"/>
+      <c r="AH24" s="60"/>
+      <c r="AI24" s="61"/>
       <c r="AJ24" s="1"/>
       <c r="AK24" s="1"/>
       <c r="AL24" s="1"/>
@@ -2280,44 +2274,44 @@
     </row>
     <row r="25" ht="19.5" customHeight="1">
       <c r="A25" s="1"/>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="C25" s="60" t="s">
+      <c r="C25" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="61"/>
-      <c r="K25" s="61"/>
-      <c r="L25" s="61"/>
-      <c r="M25" s="61"/>
-      <c r="N25" s="61"/>
-      <c r="O25" s="61"/>
-      <c r="P25" s="61"/>
-      <c r="Q25" s="61"/>
-      <c r="R25" s="61"/>
-      <c r="S25" s="62"/>
-      <c r="T25" s="62"/>
-      <c r="U25" s="62"/>
-      <c r="V25" s="62"/>
-      <c r="W25" s="62"/>
-      <c r="X25" s="62"/>
-      <c r="Y25" s="62"/>
-      <c r="Z25" s="62"/>
-      <c r="AA25" s="62"/>
-      <c r="AB25" s="62"/>
-      <c r="AC25" s="62"/>
-      <c r="AD25" s="62"/>
-      <c r="AE25" s="62"/>
-      <c r="AF25" s="62"/>
-      <c r="AG25" s="62"/>
-      <c r="AH25" s="62"/>
-      <c r="AI25" s="63"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="59"/>
+      <c r="J25" s="59"/>
+      <c r="K25" s="59"/>
+      <c r="L25" s="59"/>
+      <c r="M25" s="59"/>
+      <c r="N25" s="59"/>
+      <c r="O25" s="59"/>
+      <c r="P25" s="59"/>
+      <c r="Q25" s="59"/>
+      <c r="R25" s="59"/>
+      <c r="S25" s="60"/>
+      <c r="T25" s="60"/>
+      <c r="U25" s="60"/>
+      <c r="V25" s="60"/>
+      <c r="W25" s="60"/>
+      <c r="X25" s="60"/>
+      <c r="Y25" s="60"/>
+      <c r="Z25" s="60"/>
+      <c r="AA25" s="60"/>
+      <c r="AB25" s="60"/>
+      <c r="AC25" s="60"/>
+      <c r="AD25" s="60"/>
+      <c r="AE25" s="60"/>
+      <c r="AF25" s="60"/>
+      <c r="AG25" s="60"/>
+      <c r="AH25" s="60"/>
+      <c r="AI25" s="61"/>
       <c r="AJ25" s="1"/>
       <c r="AK25" s="1"/>
       <c r="AL25" s="1"/>
@@ -2328,42 +2322,42 @@
     </row>
     <row r="26" ht="19.5" customHeight="1">
       <c r="A26" s="1"/>
-      <c r="B26" s="51"/>
-      <c r="C26" s="60" t="s">
+      <c r="B26" s="49"/>
+      <c r="C26" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="D26" s="60"/>
-      <c r="E26" s="60"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="61"/>
-      <c r="J26" s="61"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="61"/>
-      <c r="N26" s="61"/>
-      <c r="O26" s="61"/>
-      <c r="P26" s="61"/>
-      <c r="Q26" s="61"/>
-      <c r="R26" s="61"/>
-      <c r="S26" s="62"/>
-      <c r="T26" s="62"/>
-      <c r="U26" s="62"/>
-      <c r="V26" s="62"/>
-      <c r="W26" s="62"/>
-      <c r="X26" s="62"/>
-      <c r="Y26" s="62"/>
-      <c r="Z26" s="62"/>
-      <c r="AA26" s="62"/>
-      <c r="AB26" s="62"/>
-      <c r="AC26" s="62"/>
-      <c r="AD26" s="62"/>
-      <c r="AE26" s="62"/>
-      <c r="AF26" s="62"/>
-      <c r="AG26" s="62"/>
-      <c r="AH26" s="62"/>
-      <c r="AI26" s="62"/>
+      <c r="D26" s="58"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="59"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="59"/>
+      <c r="M26" s="59"/>
+      <c r="N26" s="59"/>
+      <c r="O26" s="59"/>
+      <c r="P26" s="59"/>
+      <c r="Q26" s="59"/>
+      <c r="R26" s="59"/>
+      <c r="S26" s="60"/>
+      <c r="T26" s="60"/>
+      <c r="U26" s="60"/>
+      <c r="V26" s="60"/>
+      <c r="W26" s="60"/>
+      <c r="X26" s="60"/>
+      <c r="Y26" s="60"/>
+      <c r="Z26" s="60"/>
+      <c r="AA26" s="60"/>
+      <c r="AB26" s="60"/>
+      <c r="AC26" s="60"/>
+      <c r="AD26" s="60"/>
+      <c r="AE26" s="60"/>
+      <c r="AF26" s="60"/>
+      <c r="AG26" s="60"/>
+      <c r="AH26" s="60"/>
+      <c r="AI26" s="60"/>
       <c r="AJ26" s="1"/>
       <c r="AK26" s="1"/>
       <c r="AL26" s="1"/>
@@ -2374,44 +2368,44 @@
     </row>
     <row r="27" ht="19.5" customHeight="1">
       <c r="A27" s="1"/>
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="57" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="60" t="s">
+      <c r="C27" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="60"/>
-      <c r="E27" s="60"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="61"/>
-      <c r="J27" s="61"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="61"/>
-      <c r="N27" s="61"/>
-      <c r="O27" s="61"/>
-      <c r="P27" s="61"/>
-      <c r="Q27" s="61"/>
-      <c r="R27" s="61"/>
-      <c r="S27" s="62"/>
-      <c r="T27" s="62"/>
-      <c r="U27" s="62"/>
-      <c r="V27" s="62"/>
-      <c r="W27" s="62"/>
-      <c r="X27" s="62"/>
-      <c r="Y27" s="62"/>
-      <c r="Z27" s="62"/>
-      <c r="AA27" s="62"/>
-      <c r="AB27" s="62"/>
-      <c r="AC27" s="62"/>
-      <c r="AD27" s="62"/>
-      <c r="AE27" s="62"/>
-      <c r="AF27" s="62"/>
-      <c r="AG27" s="62"/>
-      <c r="AH27" s="62"/>
-      <c r="AI27" s="62"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="59"/>
+      <c r="N27" s="59"/>
+      <c r="O27" s="59"/>
+      <c r="P27" s="59"/>
+      <c r="Q27" s="59"/>
+      <c r="R27" s="59"/>
+      <c r="S27" s="60"/>
+      <c r="T27" s="60"/>
+      <c r="U27" s="60"/>
+      <c r="V27" s="60"/>
+      <c r="W27" s="60"/>
+      <c r="X27" s="60"/>
+      <c r="Y27" s="60"/>
+      <c r="Z27" s="60"/>
+      <c r="AA27" s="60"/>
+      <c r="AB27" s="60"/>
+      <c r="AC27" s="60"/>
+      <c r="AD27" s="60"/>
+      <c r="AE27" s="60"/>
+      <c r="AF27" s="60"/>
+      <c r="AG27" s="60"/>
+      <c r="AH27" s="60"/>
+      <c r="AI27" s="60"/>
       <c r="AJ27" s="1"/>
       <c r="AK27" s="1"/>
       <c r="AL27" s="1"/>
@@ -2422,42 +2416,42 @@
     </row>
     <row r="28" ht="19.5" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="51"/>
-      <c r="C28" s="60" t="s">
+      <c r="B28" s="49"/>
+      <c r="C28" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="60"/>
-      <c r="E28" s="60"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="61"/>
-      <c r="J28" s="61"/>
-      <c r="K28" s="61"/>
-      <c r="L28" s="61"/>
-      <c r="M28" s="61"/>
-      <c r="N28" s="61"/>
-      <c r="O28" s="61"/>
-      <c r="P28" s="61"/>
-      <c r="Q28" s="61"/>
-      <c r="R28" s="61"/>
-      <c r="S28" s="62"/>
-      <c r="T28" s="62"/>
-      <c r="U28" s="62"/>
-      <c r="V28" s="62"/>
-      <c r="W28" s="62"/>
-      <c r="X28" s="62"/>
-      <c r="Y28" s="62"/>
-      <c r="Z28" s="62"/>
-      <c r="AA28" s="62"/>
-      <c r="AB28" s="62"/>
-      <c r="AC28" s="62"/>
-      <c r="AD28" s="62"/>
-      <c r="AE28" s="62"/>
-      <c r="AF28" s="62"/>
-      <c r="AG28" s="62"/>
-      <c r="AH28" s="62"/>
-      <c r="AI28" s="62"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="58"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="59"/>
+      <c r="J28" s="59"/>
+      <c r="K28" s="59"/>
+      <c r="L28" s="59"/>
+      <c r="M28" s="59"/>
+      <c r="N28" s="59"/>
+      <c r="O28" s="59"/>
+      <c r="P28" s="59"/>
+      <c r="Q28" s="59"/>
+      <c r="R28" s="59"/>
+      <c r="S28" s="60"/>
+      <c r="T28" s="60"/>
+      <c r="U28" s="60"/>
+      <c r="V28" s="60"/>
+      <c r="W28" s="60"/>
+      <c r="X28" s="60"/>
+      <c r="Y28" s="60"/>
+      <c r="Z28" s="60"/>
+      <c r="AA28" s="60"/>
+      <c r="AB28" s="60"/>
+      <c r="AC28" s="60"/>
+      <c r="AD28" s="60"/>
+      <c r="AE28" s="60"/>
+      <c r="AF28" s="60"/>
+      <c r="AG28" s="60"/>
+      <c r="AH28" s="60"/>
+      <c r="AI28" s="60"/>
       <c r="AJ28" s="1"/>
       <c r="AK28" s="1"/>
       <c r="AL28" s="1"/>
@@ -2468,44 +2462,44 @@
     </row>
     <row r="29" ht="19.5" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="64" t="s">
+      <c r="B29" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="C29" s="60" t="s">
+      <c r="C29" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D29" s="60"/>
-      <c r="E29" s="60"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="61"/>
-      <c r="J29" s="61"/>
-      <c r="K29" s="61"/>
-      <c r="L29" s="61"/>
-      <c r="M29" s="61"/>
-      <c r="N29" s="61"/>
-      <c r="O29" s="61"/>
-      <c r="P29" s="61"/>
-      <c r="Q29" s="61"/>
-      <c r="R29" s="61"/>
-      <c r="S29" s="62"/>
-      <c r="T29" s="62"/>
-      <c r="U29" s="62"/>
-      <c r="V29" s="62"/>
-      <c r="W29" s="62"/>
-      <c r="X29" s="62"/>
-      <c r="Y29" s="62"/>
-      <c r="Z29" s="62"/>
-      <c r="AA29" s="62"/>
-      <c r="AB29" s="62"/>
-      <c r="AC29" s="62"/>
-      <c r="AD29" s="62"/>
-      <c r="AE29" s="62"/>
-      <c r="AF29" s="62"/>
-      <c r="AG29" s="62"/>
-      <c r="AH29" s="62"/>
-      <c r="AI29" s="62"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="59"/>
+      <c r="K29" s="59"/>
+      <c r="L29" s="59"/>
+      <c r="M29" s="59"/>
+      <c r="N29" s="59"/>
+      <c r="O29" s="59"/>
+      <c r="P29" s="59"/>
+      <c r="Q29" s="59"/>
+      <c r="R29" s="59"/>
+      <c r="S29" s="60"/>
+      <c r="T29" s="60"/>
+      <c r="U29" s="60"/>
+      <c r="V29" s="60"/>
+      <c r="W29" s="60"/>
+      <c r="X29" s="60"/>
+      <c r="Y29" s="60"/>
+      <c r="Z29" s="60"/>
+      <c r="AA29" s="60"/>
+      <c r="AB29" s="60"/>
+      <c r="AC29" s="60"/>
+      <c r="AD29" s="60"/>
+      <c r="AE29" s="60"/>
+      <c r="AF29" s="60"/>
+      <c r="AG29" s="60"/>
+      <c r="AH29" s="60"/>
+      <c r="AI29" s="60"/>
       <c r="AJ29" s="1"/>
       <c r="AK29" s="1"/>
       <c r="AL29" s="1"/>
@@ -2516,42 +2510,42 @@
     </row>
     <row r="30" ht="19.5" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="51"/>
-      <c r="C30" s="60" t="s">
+      <c r="B30" s="49"/>
+      <c r="C30" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="60"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="61"/>
-      <c r="J30" s="61"/>
-      <c r="K30" s="61"/>
-      <c r="L30" s="61"/>
-      <c r="M30" s="61"/>
-      <c r="N30" s="61"/>
-      <c r="O30" s="61"/>
-      <c r="P30" s="61"/>
-      <c r="Q30" s="61"/>
-      <c r="R30" s="61"/>
-      <c r="S30" s="62"/>
-      <c r="T30" s="62"/>
-      <c r="U30" s="62"/>
-      <c r="V30" s="62"/>
-      <c r="W30" s="62"/>
-      <c r="X30" s="62"/>
-      <c r="Y30" s="62"/>
-      <c r="Z30" s="62"/>
-      <c r="AA30" s="62"/>
-      <c r="AB30" s="62"/>
-      <c r="AC30" s="62"/>
-      <c r="AD30" s="62"/>
-      <c r="AE30" s="62"/>
-      <c r="AF30" s="62"/>
-      <c r="AG30" s="62"/>
-      <c r="AH30" s="62"/>
-      <c r="AI30" s="61"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="58"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="59"/>
+      <c r="J30" s="59"/>
+      <c r="K30" s="59"/>
+      <c r="L30" s="59"/>
+      <c r="M30" s="59"/>
+      <c r="N30" s="59"/>
+      <c r="O30" s="59"/>
+      <c r="P30" s="59"/>
+      <c r="Q30" s="59"/>
+      <c r="R30" s="59"/>
+      <c r="S30" s="60"/>
+      <c r="T30" s="60"/>
+      <c r="U30" s="60"/>
+      <c r="V30" s="60"/>
+      <c r="W30" s="60"/>
+      <c r="X30" s="60"/>
+      <c r="Y30" s="60"/>
+      <c r="Z30" s="60"/>
+      <c r="AA30" s="60"/>
+      <c r="AB30" s="60"/>
+      <c r="AC30" s="60"/>
+      <c r="AD30" s="60"/>
+      <c r="AE30" s="60"/>
+      <c r="AF30" s="60"/>
+      <c r="AG30" s="60"/>
+      <c r="AH30" s="60"/>
+      <c r="AI30" s="59"/>
       <c r="AJ30" s="1"/>
       <c r="AK30" s="1"/>
       <c r="AL30" s="1"/>
@@ -2565,41 +2559,41 @@
       <c r="B31" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C31" s="60" t="s">
+      <c r="C31" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D31" s="60"/>
-      <c r="E31" s="60"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="61"/>
-      <c r="J31" s="61"/>
-      <c r="K31" s="61"/>
-      <c r="L31" s="61"/>
-      <c r="M31" s="61"/>
-      <c r="N31" s="61"/>
-      <c r="O31" s="61"/>
-      <c r="P31" s="61"/>
-      <c r="Q31" s="61"/>
-      <c r="R31" s="61"/>
-      <c r="S31" s="62"/>
-      <c r="T31" s="62"/>
-      <c r="U31" s="62"/>
-      <c r="V31" s="62"/>
-      <c r="W31" s="62"/>
-      <c r="X31" s="62"/>
-      <c r="Y31" s="62"/>
-      <c r="Z31" s="62"/>
-      <c r="AA31" s="62"/>
-      <c r="AB31" s="62"/>
-      <c r="AC31" s="62"/>
-      <c r="AD31" s="62"/>
-      <c r="AE31" s="62"/>
-      <c r="AF31" s="62"/>
-      <c r="AG31" s="62"/>
-      <c r="AH31" s="62"/>
-      <c r="AI31" s="61"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="58"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="59"/>
+      <c r="J31" s="59"/>
+      <c r="K31" s="59"/>
+      <c r="L31" s="59"/>
+      <c r="M31" s="59"/>
+      <c r="N31" s="59"/>
+      <c r="O31" s="59"/>
+      <c r="P31" s="59"/>
+      <c r="Q31" s="59"/>
+      <c r="R31" s="59"/>
+      <c r="S31" s="60"/>
+      <c r="T31" s="60"/>
+      <c r="U31" s="60"/>
+      <c r="V31" s="60"/>
+      <c r="W31" s="60"/>
+      <c r="X31" s="60"/>
+      <c r="Y31" s="60"/>
+      <c r="Z31" s="60"/>
+      <c r="AA31" s="60"/>
+      <c r="AB31" s="60"/>
+      <c r="AC31" s="60"/>
+      <c r="AD31" s="60"/>
+      <c r="AE31" s="60"/>
+      <c r="AF31" s="60"/>
+      <c r="AG31" s="60"/>
+      <c r="AH31" s="60"/>
+      <c r="AI31" s="59"/>
       <c r="AJ31" s="1"/>
       <c r="AK31" s="1"/>
       <c r="AL31" s="1"/>
@@ -2610,42 +2604,42 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="51"/>
-      <c r="C32" s="60" t="s">
+      <c r="B32" s="49"/>
+      <c r="C32" s="58" t="s">
         <v>51</v>
       </c>
-      <c r="D32" s="60"/>
-      <c r="E32" s="60"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="54"/>
-      <c r="H32" s="54"/>
-      <c r="I32" s="54"/>
-      <c r="J32" s="54"/>
-      <c r="K32" s="63"/>
-      <c r="L32" s="63"/>
-      <c r="M32" s="63"/>
-      <c r="N32" s="63"/>
-      <c r="O32" s="63"/>
-      <c r="P32" s="63"/>
-      <c r="Q32" s="63"/>
-      <c r="R32" s="63"/>
-      <c r="S32" s="63"/>
-      <c r="T32" s="63"/>
-      <c r="U32" s="63"/>
-      <c r="V32" s="63"/>
-      <c r="W32" s="63"/>
-      <c r="X32" s="63"/>
-      <c r="Y32" s="63"/>
-      <c r="Z32" s="63"/>
-      <c r="AA32" s="63"/>
-      <c r="AB32" s="63"/>
-      <c r="AC32" s="63"/>
-      <c r="AD32" s="63"/>
-      <c r="AE32" s="63"/>
-      <c r="AF32" s="63"/>
-      <c r="AG32" s="63"/>
-      <c r="AH32" s="63"/>
-      <c r="AI32" s="63"/>
+      <c r="D32" s="58"/>
+      <c r="E32" s="58"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="52"/>
+      <c r="K32" s="61"/>
+      <c r="L32" s="61"/>
+      <c r="M32" s="61"/>
+      <c r="N32" s="61"/>
+      <c r="O32" s="61"/>
+      <c r="P32" s="61"/>
+      <c r="Q32" s="61"/>
+      <c r="R32" s="61"/>
+      <c r="S32" s="61"/>
+      <c r="T32" s="61"/>
+      <c r="U32" s="61"/>
+      <c r="V32" s="61"/>
+      <c r="W32" s="61"/>
+      <c r="X32" s="61"/>
+      <c r="Y32" s="61"/>
+      <c r="Z32" s="61"/>
+      <c r="AA32" s="61"/>
+      <c r="AB32" s="61"/>
+      <c r="AC32" s="61"/>
+      <c r="AD32" s="61"/>
+      <c r="AE32" s="61"/>
+      <c r="AF32" s="61"/>
+      <c r="AG32" s="61"/>
+      <c r="AH32" s="61"/>
+      <c r="AI32" s="61"/>
       <c r="AJ32" s="1"/>
       <c r="AK32" s="1"/>
       <c r="AL32" s="1"/>
@@ -2700,23 +2694,23 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="1"/>
-      <c r="B34" s="65" t="s">
+      <c r="B34" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="C34" s="66"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="67"/>
-      <c r="H34" s="67"/>
-      <c r="I34" s="67"/>
-      <c r="J34" s="67"/>
-      <c r="K34" s="67"/>
-      <c r="L34" s="67"/>
-      <c r="M34" s="67"/>
-      <c r="N34" s="67"/>
-      <c r="O34" s="67"/>
-      <c r="P34" s="67"/>
+      <c r="C34" s="64"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
+      <c r="L34" s="65"/>
+      <c r="M34" s="65"/>
+      <c r="N34" s="65"/>
+      <c r="O34" s="65"/>
+      <c r="P34" s="65"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
       <c r="S34" s="1"/>
@@ -2746,23 +2740,23 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="65" t="s">
+      <c r="B35" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="66"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="66"/>
-      <c r="F35" s="67"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
-      <c r="K35" s="67"/>
-      <c r="L35" s="67"/>
-      <c r="M35" s="67"/>
-      <c r="N35" s="67"/>
-      <c r="O35" s="67"/>
-      <c r="P35" s="67"/>
+      <c r="C35" s="64"/>
+      <c r="D35" s="64"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="65"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="65"/>
+      <c r="J35" s="65"/>
+      <c r="K35" s="65"/>
+      <c r="L35" s="65"/>
+      <c r="M35" s="65"/>
+      <c r="N35" s="65"/>
+      <c r="O35" s="65"/>
+      <c r="P35" s="65"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
@@ -2793,20 +2787,20 @@
     <row r="36" ht="4.5" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="68"/>
-      <c r="D36" s="68"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="67"/>
-      <c r="H36" s="67"/>
-      <c r="I36" s="67"/>
-      <c r="J36" s="67"/>
-      <c r="K36" s="67"/>
-      <c r="L36" s="67"/>
-      <c r="M36" s="67"/>
-      <c r="N36" s="67"/>
-      <c r="O36" s="67"/>
-      <c r="P36" s="67"/>
+      <c r="C36" s="66"/>
+      <c r="D36" s="66"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="65"/>
+      <c r="K36" s="65"/>
+      <c r="L36" s="65"/>
+      <c r="M36" s="65"/>
+      <c r="N36" s="65"/>
+      <c r="O36" s="65"/>
+      <c r="P36" s="65"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
@@ -3144,9 +3138,9 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="1"/>
-      <c r="B44" s="69"/>
-      <c r="C44" s="69"/>
-      <c r="D44" s="69"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="67"/>
+      <c r="D44" s="67"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -3188,9 +3182,9 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="9"/>
-      <c r="B45" s="70"/>
-      <c r="C45" s="71"/>
-      <c r="D45" s="71"/>
+      <c r="B45" s="68"/>
+      <c r="C45" s="69"/>
+      <c r="D45" s="69"/>
       <c r="E45" s="17"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -3232,9 +3226,9 @@
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="9"/>
-      <c r="B46" s="72"/>
-      <c r="C46" s="73"/>
-      <c r="D46" s="74"/>
+      <c r="B46" s="70"/>
+      <c r="C46" s="71"/>
+      <c r="D46" s="72"/>
       <c r="E46" s="17"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -3276,9 +3270,9 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="9"/>
-      <c r="B47" s="75"/>
-      <c r="C47" s="73"/>
-      <c r="D47" s="76"/>
+      <c r="B47" s="73"/>
+      <c r="C47" s="71"/>
+      <c r="D47" s="74"/>
       <c r="E47" s="17"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -3320,9 +3314,9 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="9"/>
-      <c r="B48" s="77"/>
-      <c r="C48" s="73"/>
-      <c r="D48" s="76"/>
+      <c r="B48" s="75"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="74"/>
       <c r="E48" s="17"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -3364,9 +3358,9 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="9"/>
-      <c r="B49" s="75"/>
-      <c r="C49" s="73"/>
-      <c r="D49" s="74"/>
+      <c r="B49" s="73"/>
+      <c r="C49" s="71"/>
+      <c r="D49" s="72"/>
       <c r="E49" s="17"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -3408,9 +3402,9 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="9"/>
-      <c r="B50" s="72"/>
-      <c r="C50" s="73"/>
-      <c r="D50" s="76"/>
+      <c r="B50" s="70"/>
+      <c r="C50" s="71"/>
+      <c r="D50" s="74"/>
       <c r="E50" s="17"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -3452,9 +3446,9 @@
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="9"/>
-      <c r="B51" s="75"/>
-      <c r="C51" s="78"/>
-      <c r="D51" s="78"/>
+      <c r="B51" s="73"/>
+      <c r="C51" s="76"/>
+      <c r="D51" s="76"/>
       <c r="E51" s="17"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -3496,9 +3490,9 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="9"/>
-      <c r="B52" s="72"/>
-      <c r="C52" s="78"/>
-      <c r="D52" s="78"/>
+      <c r="B52" s="70"/>
+      <c r="C52" s="76"/>
+      <c r="D52" s="76"/>
       <c r="E52" s="17"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -3540,9 +3534,9 @@
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="9"/>
-      <c r="B53" s="75"/>
-      <c r="C53" s="78"/>
-      <c r="D53" s="78"/>
+      <c r="B53" s="73"/>
+      <c r="C53" s="76"/>
+      <c r="D53" s="76"/>
       <c r="E53" s="17"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -3584,9 +3578,9 @@
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="9"/>
-      <c r="B54" s="72"/>
-      <c r="C54" s="78"/>
-      <c r="D54" s="78"/>
+      <c r="B54" s="70"/>
+      <c r="C54" s="76"/>
+      <c r="D54" s="76"/>
       <c r="E54" s="17"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -45340,58 +45334,58 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="E13:G14"/>
+    <mergeCell ref="K15:R15"/>
+    <mergeCell ref="S15:S17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="X15:X17"/>
+    <mergeCell ref="Y15:Y17"/>
+    <mergeCell ref="Z15:Z17"/>
+    <mergeCell ref="AA15:AA17"/>
+    <mergeCell ref="AB15:AB17"/>
+    <mergeCell ref="AD15:AD17"/>
+    <mergeCell ref="AE15:AF15"/>
+    <mergeCell ref="AE16:AE17"/>
+    <mergeCell ref="AF16:AF17"/>
     <mergeCell ref="H13:J14"/>
     <mergeCell ref="K13:R13"/>
     <mergeCell ref="S13:AC13"/>
-    <mergeCell ref="AD13:AF14"/>
     <mergeCell ref="AG13:AG17"/>
     <mergeCell ref="AH13:AH17"/>
     <mergeCell ref="AI13:AI17"/>
+    <mergeCell ref="V14:AB14"/>
     <mergeCell ref="K14:R14"/>
     <mergeCell ref="S14:U14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="K15:R15"/>
-    <mergeCell ref="V14:AB14"/>
+    <mergeCell ref="AD13:AF14"/>
     <mergeCell ref="AC14:AC17"/>
-    <mergeCell ref="V15:V17"/>
-    <mergeCell ref="W15:W17"/>
-    <mergeCell ref="X15:X17"/>
-    <mergeCell ref="Y15:Y17"/>
-    <mergeCell ref="Z15:Z17"/>
     <mergeCell ref="C9:K9"/>
     <mergeCell ref="C10:K10"/>
     <mergeCell ref="C11:K11"/>
     <mergeCell ref="B13:B17"/>
     <mergeCell ref="C13:C17"/>
-    <mergeCell ref="AE15:AF15"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:E35"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="E13:G14"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="T15:T17"/>
+    <mergeCell ref="U15:U17"/>
+    <mergeCell ref="V15:V17"/>
+    <mergeCell ref="W15:W17"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B31:B32"/>
-    <mergeCell ref="S15:S17"/>
-    <mergeCell ref="T15:T17"/>
-    <mergeCell ref="AA15:AA17"/>
-    <mergeCell ref="AB15:AB17"/>
-    <mergeCell ref="U15:U17"/>
-    <mergeCell ref="AD15:AD17"/>
-    <mergeCell ref="D13:D17"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:E35"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:G17"/>
     <mergeCell ref="E16:E17"/>
     <mergeCell ref="F16:F17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:N16"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="AE16:AE17"/>
-    <mergeCell ref="AF16:AF17"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>